<commit_message>
Added 'nfhs5 analytic dataset' variables
</commit_message>
<xml_diff>
--- a/data/India HbA1c Prediction Variable List.xlsx
+++ b/data/India HbA1c Prediction Variable List.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\india_hba1c_prediction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B46CD0-406E-4A0B-AC3B-A2B953468EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECD4D76-F486-4DD0-BE2E-F80A1E827DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-15840" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-14520" windowWidth="16440" windowHeight="28440" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nfhs5 variables" sheetId="1" r:id="rId1"/>
     <sheet name="carrs variables" sheetId="5" r:id="rId2"/>
     <sheet name="carrs analytic dataset" sheetId="6" r:id="rId3"/>
-    <sheet name="mapnfhs5_sdist" sheetId="3" r:id="rId4"/>
-    <sheet name="mapnfhs5_v024" sheetId="2" r:id="rId5"/>
+    <sheet name="nfhs5 analytic dataset" sheetId="7" r:id="rId4"/>
+    <sheet name="mapnfhs5_sdist" sheetId="3" r:id="rId5"/>
+    <sheet name="mapnfhs5_v024" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3389" uniqueCount="1477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="1556">
   <si>
     <t>label</t>
   </si>
@@ -4077,9 +4078,6 @@
     <t>hv226</t>
   </si>
   <si>
-    <t>sh45</t>
-  </si>
-  <si>
     <t>hv209</t>
   </si>
   <si>
@@ -4498,6 +4496,246 @@
   </si>
   <si>
     <t>Married (1: Yes, 0: No)</t>
+  </si>
+  <si>
+    <t>interview</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>diagnosed_dm</t>
+  </si>
+  <si>
+    <t>treated_dm</t>
+  </si>
+  <si>
+    <t>diagnosed_bp</t>
+  </si>
+  <si>
+    <t>treated_bp</t>
+  </si>
+  <si>
+    <t>bmi_underweight</t>
+  </si>
+  <si>
+    <t>bmi_overweight</t>
+  </si>
+  <si>
+    <t>bmi_obese</t>
+  </si>
+  <si>
+    <t>fasting</t>
+  </si>
+  <si>
+    <t>sbp</t>
+  </si>
+  <si>
+    <t>dbp</t>
+  </si>
+  <si>
+    <t>na_caste</t>
+  </si>
+  <si>
+    <t>na_education</t>
+  </si>
+  <si>
+    <t>bmi_category</t>
+  </si>
+  <si>
+    <t>highwc</t>
+  </si>
+  <si>
+    <t>waist_hip</t>
+  </si>
+  <si>
+    <t>highwhr</t>
+  </si>
+  <si>
+    <t>age_category</t>
+  </si>
+  <si>
+    <t>swealthq_ur</t>
+  </si>
+  <si>
+    <t>swealths_ur</t>
+  </si>
+  <si>
+    <t>age_category10</t>
+  </si>
+  <si>
+    <t>age_category5</t>
+  </si>
+  <si>
+    <t>Male or Female</t>
+  </si>
+  <si>
+    <t>Cluster (v001)</t>
+  </si>
+  <si>
+    <t>Household ID (v002)</t>
+  </si>
+  <si>
+    <t>Individual line number (v003)</t>
+  </si>
+  <si>
+    <t>Sample weight for household (v005)</t>
+  </si>
+  <si>
+    <t>Primary sampling unit (v021)</t>
+  </si>
+  <si>
+    <t>Strata for survey design (v022)</t>
+  </si>
+  <si>
+    <t>State in NFHS-5 (v024)</t>
+  </si>
+  <si>
+    <t>Urban or Rural (v025)</t>
+  </si>
+  <si>
+    <t>No education, Primary, Secondary, Higher</t>
+  </si>
+  <si>
+    <t>Hindu, Muslim, Other</t>
+  </si>
+  <si>
+    <t>Schooling in single years (v133)</t>
+  </si>
+  <si>
+    <t>National wealth quintile (v190)</t>
+  </si>
+  <si>
+    <t>National wealth index (v191)</t>
+  </si>
+  <si>
+    <t>Number of children (v218)</t>
+  </si>
+  <si>
+    <t>Height (cm)</t>
+  </si>
+  <si>
+    <t>BMI (kg/m2)</t>
+  </si>
+  <si>
+    <t>Currently pregnant (v454)</t>
+  </si>
+  <si>
+    <t>State wealth quintile</t>
+  </si>
+  <si>
+    <t>State urban wealth quintile</t>
+  </si>
+  <si>
+    <t>State urban wealth index</t>
+  </si>
+  <si>
+    <t>State rural wealth quintile</t>
+  </si>
+  <si>
+    <t>State rural wealth index</t>
+  </si>
+  <si>
+    <t>Wealth quintile regional</t>
+  </si>
+  <si>
+    <t>Wealth index regional</t>
+  </si>
+  <si>
+    <t>State wealth index</t>
+  </si>
+  <si>
+    <t>ICMR criterion SBP</t>
+  </si>
+  <si>
+    <t>Corresponding DBP to SBP</t>
+  </si>
+  <si>
+    <t>Hypertension (Self-reported or &gt;=140/90)</t>
+  </si>
+  <si>
+    <t>State wealth quintile - regional</t>
+  </si>
+  <si>
+    <t>State wealth index - regional</t>
+  </si>
+  <si>
+    <t>Age category (18-29, 30-39, 40-49…)</t>
+  </si>
+  <si>
+    <t>Age category (15-19, 20-24, 25-29,…)</t>
+  </si>
+  <si>
+    <t>Age category (18-39, 40-64, 65+)</t>
+  </si>
+  <si>
+    <t>Waist to hip ratio</t>
+  </si>
+  <si>
+    <t>BMI category (Underweight, Normal, Overweight, Obesity)</t>
+  </si>
+  <si>
+    <t>High waist circumference</t>
+  </si>
+  <si>
+    <t>High waist to hip ratio</t>
+  </si>
+  <si>
+    <t>is_malesample</t>
+  </si>
+  <si>
+    <t>nadultsmeasured</t>
+  </si>
+  <si>
+    <t>is_evermarriedsample</t>
+  </si>
+  <si>
+    <t>hv205</t>
+  </si>
+  <si>
+    <t>Ever married sample (hv020)</t>
+  </si>
+  <si>
+    <t>Male sample (hv027)</t>
+  </si>
+  <si>
+    <t>Total adults measured (hv041)</t>
+  </si>
+  <si>
+    <t>Kitchen (hv242)</t>
+  </si>
+  <si>
+    <t>Fuel (hv226)</t>
+  </si>
+  <si>
+    <t>Water (hv201)</t>
+  </si>
+  <si>
+    <t>Toilet (hv205)</t>
+  </si>
+  <si>
+    <t>Tv (sh50j)</t>
+  </si>
+  <si>
+    <t>Fridge (hv209)</t>
+  </si>
+  <si>
+    <t>Wmachine (sh50r)</t>
+  </si>
+  <si>
+    <t>Mobile (hv243a)</t>
+  </si>
+  <si>
+    <t>Computer (hv243e)</t>
+  </si>
+  <si>
+    <t>Car (hv212)</t>
+  </si>
+  <si>
+    <t>Scooter (hv211)</t>
+  </si>
+  <si>
+    <t>Bicycle (hv210)</t>
   </si>
 </sst>
 </file>
@@ -5056,11 +5294,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="B117" sqref="B117:B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5117,9 +5355,6 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -5154,9 +5389,6 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -5174,9 +5406,6 @@
       <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -5240,9 +5469,6 @@
       <c r="F8" t="s">
         <v>36</v>
       </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -5263,9 +5489,6 @@
       <c r="F9" t="s">
         <v>40</v>
       </c>
-      <c r="G9" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -5309,9 +5532,6 @@
       <c r="F11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -5432,9 +5652,6 @@
       <c r="F17" t="s">
         <v>79</v>
       </c>
-      <c r="G17" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -7098,6 +7315,9 @@
       <c r="A117" t="s">
         <v>502</v>
       </c>
+      <c r="B117" t="s">
+        <v>1539</v>
+      </c>
       <c r="G117" t="s">
         <v>503</v>
       </c>
@@ -7106,6 +7326,9 @@
       <c r="A118" t="s">
         <v>504</v>
       </c>
+      <c r="B118" t="s">
+        <v>1537</v>
+      </c>
       <c r="G118" t="s">
         <v>505</v>
       </c>
@@ -7114,6 +7337,9 @@
       <c r="A119" t="s">
         <v>506</v>
       </c>
+      <c r="B119" t="s">
+        <v>1538</v>
+      </c>
       <c r="G119" t="s">
         <v>507</v>
       </c>
@@ -7148,7 +7374,7 @@
         <v>1302</v>
       </c>
       <c r="G122" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -7159,7 +7385,7 @@
         <v>1303</v>
       </c>
       <c r="G123" t="s">
-        <v>1336</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
@@ -7181,7 +7407,7 @@
         <v>1305</v>
       </c>
       <c r="G125" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -7249,7 +7475,7 @@
         <v>1312</v>
       </c>
       <c r="G132" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
@@ -7260,7 +7486,7 @@
         <v>1313</v>
       </c>
       <c r="G133" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
@@ -7271,7 +7497,7 @@
         <v>1314</v>
       </c>
       <c r="G134" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
   </sheetData>
@@ -7344,7 +7570,7 @@
         <v>1254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -7386,7 +7612,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1259</v>
@@ -7480,13 +7706,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B12" t="s">
         <v>1345</v>
       </c>
-      <c r="B12" t="s">
-        <v>1346</v>
-      </c>
       <c r="C12" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="D12" t="s">
         <v>1281</v>
@@ -7700,24 +7926,24 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B35" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="E35" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="G35" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B36" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="E36" t="s">
         <v>1264</v>
@@ -7728,51 +7954,51 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B37" t="s">
         <v>1406</v>
       </c>
-      <c r="B37" t="s">
+      <c r="E37" t="s">
         <v>1407</v>
-      </c>
-      <c r="E37" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B38" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C38" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B39" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B40" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="C40" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B41" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="E41" t="s">
         <v>1276</v>
@@ -7780,10 +8006,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B42" t="s">
         <v>1361</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1362</v>
       </c>
       <c r="E42" t="s">
         <v>1265</v>
@@ -7791,10 +8017,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="B43" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E43" t="s">
         <v>1263</v>
@@ -7802,73 +8028,73 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="B44" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C44" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B45" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C45" t="s">
         <v>1393</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1394</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B46" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="E46" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="B47" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E47" t="s">
         <v>1400</v>
-      </c>
-      <c r="E47" t="s">
-        <v>1401</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B48" t="s">
         <v>1403</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E48" t="s">
         <v>1404</v>
-      </c>
-      <c r="E48" t="s">
-        <v>1405</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B49" t="s">
         <v>1410</v>
       </c>
-      <c r="B49" t="s">
+      <c r="E49" t="s">
         <v>1411</v>
-      </c>
-      <c r="E49" t="s">
-        <v>1412</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>384</v>
@@ -7882,7 +8108,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>399</v>
@@ -7896,10 +8122,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="E52" t="s">
         <v>1278</v>
@@ -7907,10 +8133,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="E53" t="s">
         <v>1277</v>
@@ -8012,10 +8238,10 @@
         <v>255</v>
       </c>
       <c r="C65" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="F65" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -8026,10 +8252,10 @@
         <v>260</v>
       </c>
       <c r="C66" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="F66" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -8076,79 +8302,79 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B70" t="s">
         <v>1370</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F70" t="s">
         <v>1371</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1396</v>
-      </c>
-      <c r="F70" t="s">
-        <v>1372</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B71" t="s">
         <v>1373</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>1374</v>
       </c>
-      <c r="C71" t="s">
-        <v>1375</v>
-      </c>
       <c r="F71" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B72" t="s">
         <v>1376</v>
       </c>
-      <c r="B72" t="s">
-        <v>1377</v>
-      </c>
       <c r="C72" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="F72" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C73" t="s">
         <v>1378</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1382</v>
-      </c>
-      <c r="C73" t="s">
-        <v>1379</v>
       </c>
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B74" t="s">
         <v>1380</v>
       </c>
-      <c r="B74" t="s">
-        <v>1381</v>
-      </c>
       <c r="C74" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B75" t="s">
         <v>1384</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>1385</v>
-      </c>
-      <c r="C75" t="s">
-        <v>1386</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -8214,7 +8440,7 @@
         <v>326</v>
       </c>
       <c r="B82" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="E82" t="s">
         <v>1262</v>
@@ -8222,10 +8448,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B83" t="s">
         <v>1462</v>
-      </c>
-      <c r="B83" t="s">
-        <v>1463</v>
       </c>
       <c r="E83" t="s">
         <v>1299</v>
@@ -8439,19 +8665,19 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B106" t="s">
         <v>1347</v>
       </c>
-      <c r="B106" t="s">
-        <v>1348</v>
-      </c>
       <c r="C106" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="D106" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="F106" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -8785,8 +9011,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D18BEB6-56B3-4D14-B012-CA4E5B8591AD}">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8797,13 +9024,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -8811,7 +9038,7 @@
         <v>1257</v>
       </c>
       <c r="B2" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -8819,7 +9046,7 @@
         <v>1258</v>
       </c>
       <c r="B3" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -8827,7 +9054,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -8835,7 +9062,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -8843,7 +9070,7 @@
         <v>1260</v>
       </c>
       <c r="B6" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -8851,7 +9078,7 @@
         <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -8859,7 +9086,7 @@
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -8984,42 +9211,42 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B24" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B25" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B26" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B27" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B28" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -9027,7 +9254,7 @@
         <v>1288</v>
       </c>
       <c r="B29" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -9035,7 +9262,7 @@
         <v>1289</v>
       </c>
       <c r="B30" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -9043,15 +9270,15 @@
         <v>1290</v>
       </c>
       <c r="B31" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B32" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -9059,7 +9286,7 @@
         <v>295</v>
       </c>
       <c r="B33" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -9067,7 +9294,7 @@
         <v>274</v>
       </c>
       <c r="B34" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -9075,7 +9302,7 @@
         <v>279</v>
       </c>
       <c r="B35" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -9083,7 +9310,7 @@
         <v>255</v>
       </c>
       <c r="B36" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -9091,47 +9318,47 @@
         <v>260</v>
       </c>
       <c r="B37" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B38" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="B39" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B40" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B41" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="B42" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -9139,7 +9366,7 @@
         <v>439</v>
       </c>
       <c r="B43" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -9147,7 +9374,7 @@
         <v>454</v>
       </c>
       <c r="B44" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -9155,7 +9382,7 @@
         <v>469</v>
       </c>
       <c r="B45" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -9163,7 +9390,7 @@
         <v>444</v>
       </c>
       <c r="B46" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -9171,7 +9398,7 @@
         <v>459</v>
       </c>
       <c r="B47" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -9179,7 +9406,7 @@
         <v>474</v>
       </c>
       <c r="B48" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -9192,18 +9419,18 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B50" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="B51" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -9211,15 +9438,15 @@
         <v>1291</v>
       </c>
       <c r="B52" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="B53" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -9227,7 +9454,7 @@
         <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -9235,7 +9462,7 @@
         <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -9243,7 +9470,7 @@
         <v>92</v>
       </c>
       <c r="B56" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -9251,7 +9478,7 @@
         <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -9259,15 +9486,15 @@
         <v>324</v>
       </c>
       <c r="B58" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="B59" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -9275,95 +9502,95 @@
         <v>319</v>
       </c>
       <c r="B60" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="B61" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B62" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B63" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B64" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="B65" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="B66" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="B67" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B68" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="B69" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B70" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B71" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -9371,7 +9598,7 @@
         <v>384</v>
       </c>
       <c r="B72" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -9379,23 +9606,23 @@
         <v>399</v>
       </c>
       <c r="B73" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B74" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B75" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -9403,23 +9630,23 @@
         <v>1259</v>
       </c>
       <c r="B76" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B77" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B78" t="s">
         <v>1456</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1457</v>
       </c>
     </row>
   </sheetData>
@@ -9434,6 +9661,1016 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD51443D-084D-41B3-9F65-7191FF05B41C}">
+  <dimension ref="A1:B153"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>499</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>255</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>260</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>295</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>300</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>439</v>
+      </c>
+      <c r="B80" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>444</v>
+      </c>
+      <c r="B81" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>454</v>
+      </c>
+      <c r="B86" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>459</v>
+      </c>
+      <c r="B87" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>469</v>
+      </c>
+      <c r="B89" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>474</v>
+      </c>
+      <c r="B90" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>479</v>
+      </c>
+      <c r="B91" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>484</v>
+      </c>
+      <c r="B92" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>148</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>156</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>161</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>171</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>142</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>145</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>153</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>324</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B132" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B135" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B148" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B149" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86B8A38-A044-42AF-9323-B37338C091AB}">
   <dimension ref="A1:F708"/>
   <sheetViews>
@@ -23611,7 +24848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2ECD17D-6C48-46CE-B48D-72015CCAE7B8}">
   <dimension ref="A1:D38"/>
   <sheetViews>

</xml_diff>